<commit_message>
Optimize and adjust the mobile interface
</commit_message>
<xml_diff>
--- a/WebRoot/oem/heichao/locale/locale-en.xlsx
+++ b/WebRoot/oem/heichao/locale/locale-en.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2260" uniqueCount="2186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2264" uniqueCount="2190">
   <si>
     <t>myself</t>
   </si>
@@ -8407,6 +8407,22 @@
   </si>
   <si>
     <t>CBM Production Intelligent Monitoring System V9.3 mainly focuses on oil well intelligent analysis on the basis of collection and control. The module includes real-time monitoring, historical query, production report, fault query, log query, computing maintenance, driver configuration, rights management, device management, and system configuration. The system applies big data analysis method to carry out statistical analysis of key production indicators, find abnormal production Wells in time, tap production potential Wells, and improve the control ability of target blocks and individual Wells.</t>
+  </si>
+  <si>
+    <t>userNameEmpty</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The username cannot be empty</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>passwordEmpty</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The password cannot be empty</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -8486,7 +8502,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -8505,6 +8521,10 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -8806,10 +8826,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C107"/>
+  <dimension ref="A1:D109"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -8818,7 +8838,7 @@
     <col min="3" max="3" width="50.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -8829,7 +8849,7 @@
         <v>2183</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -8840,7 +8860,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -8851,8 +8871,8 @@
         <v>1959</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="12">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -8862,323 +8882,324 @@
         <v>971</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+    <row r="5" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="12">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="14" t="s">
+        <v>2186</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>2187</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="12">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>972</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
+    <row r="7" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="12">
+        <v>6</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>2188</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>2189</v>
+      </c>
+      <c r="D7" s="15"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="12">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>973</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="12">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>974</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="12">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="12">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>1960</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>1961</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="12">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>1802</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>1801</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>11</v>
-      </c>
-      <c r="B12" s="1" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>1804</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>1803</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>12</v>
-      </c>
-      <c r="B13" s="1" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="12">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>13</v>
-      </c>
-      <c r="B14" s="1" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="12">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>1621</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>1620</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>14</v>
-      </c>
-      <c r="B15" s="1" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="12">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>975</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>15</v>
-      </c>
-      <c r="B16" s="1" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="12">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>16</v>
-      </c>
-      <c r="B17" s="1" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="12">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>1940</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>1939</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>17</v>
-      </c>
-      <c r="B18" s="1" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="12">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>2038</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>2037</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>18</v>
-      </c>
-      <c r="B19" s="1" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="12">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>976</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>19</v>
-      </c>
-      <c r="B20" s="1" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="12">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>977</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>20</v>
-      </c>
-      <c r="B21" s="1" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="12">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>978</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>21</v>
-      </c>
-      <c r="B22" s="1" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="12">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>979</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>22</v>
-      </c>
-      <c r="B23" s="1" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="12">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>980</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>23</v>
-      </c>
-      <c r="B24" s="1" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="12">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>24</v>
-      </c>
-      <c r="B25" s="1" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="12">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
-        <v>25</v>
-      </c>
-      <c r="B26" s="1" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="12">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
-        <v>26</v>
-      </c>
-      <c r="B27" s="1" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="12">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>981</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
-        <v>27</v>
-      </c>
-      <c r="B28" s="1" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="12">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C30" s="1" t="s">
         <v>1986</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
-        <v>28</v>
-      </c>
-      <c r="B29" s="1" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="12">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
-        <v>29</v>
-      </c>
-      <c r="B30" s="1" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="12">
+        <v>31</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <v>30</v>
-      </c>
-      <c r="B31" s="1" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="12">
+        <v>32</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>148</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
-        <v>31</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
-        <v>32</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>2018</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>2019</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -9186,10 +9207,10 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>52</v>
+        <v>150</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>982</v>
+        <v>149</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -9197,10 +9218,10 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>119</v>
+        <v>2018</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>983</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -9208,10 +9229,10 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>141</v>
+        <v>52</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -9219,10 +9240,10 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>367</v>
+        <v>119</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -9230,10 +9251,10 @@
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>368</v>
+        <v>141</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -9241,10 +9262,10 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>130</v>
+        <v>367</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -9252,10 +9273,10 @@
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>299</v>
+        <v>368</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -9263,10 +9284,10 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>298</v>
+        <v>130</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -9274,10 +9295,10 @@
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>131</v>
+        <v>299</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -9285,10 +9306,10 @@
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>137</v>
+        <v>298</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>140</v>
+        <v>989</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -9296,10 +9317,10 @@
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -9307,10 +9328,10 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>992</v>
+        <v>140</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -9318,10 +9339,10 @@
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -9329,10 +9350,10 @@
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -9340,10 +9361,10 @@
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>1964</v>
+        <v>132</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1965</v>
+        <v>993</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -9351,10 +9372,10 @@
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>917</v>
+        <v>142</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -9362,10 +9383,10 @@
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>918</v>
+        <v>1964</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>996</v>
+        <v>1965</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -9373,10 +9394,10 @@
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>133</v>
+        <v>917</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -9384,10 +9405,10 @@
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>134</v>
+        <v>918</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -9395,10 +9416,10 @@
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -9406,10 +9427,10 @@
         <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>31</v>
+        <v>134</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -9417,10 +9438,10 @@
         <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>2052</v>
+        <v>135</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>2053</v>
+        <v>999</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -9428,10 +9449,10 @@
         <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>311</v>
+        <v>31</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>1900</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -9439,10 +9460,10 @@
         <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>4</v>
+        <v>2052</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>1898</v>
+        <v>2053</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -9450,10 +9471,10 @@
         <v>57</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>5</v>
+        <v>311</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>1899</v>
+        <v>1900</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -9461,10 +9482,10 @@
         <v>58</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>1897</v>
+        <v>1898</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -9472,10 +9493,10 @@
         <v>59</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>1901</v>
+        <v>1899</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -9483,10 +9504,10 @@
         <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>312</v>
+        <v>6</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>1902</v>
+        <v>1897</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -9494,10 +9515,10 @@
         <v>61</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>1902</v>
+        <v>1901</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -9505,10 +9526,10 @@
         <v>62</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>231</v>
+        <v>312</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>234</v>
+        <v>1902</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -9516,10 +9537,10 @@
         <v>63</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>232</v>
+        <v>23</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>245</v>
+        <v>1902</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -9527,10 +9548,10 @@
         <v>64</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>1001</v>
+        <v>234</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -9538,10 +9559,10 @@
         <v>65</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>235</v>
+        <v>245</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -9549,10 +9570,10 @@
         <v>66</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>1966</v>
+        <v>233</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>250</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -9560,10 +9581,10 @@
         <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>1002</v>
+        <v>235</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -9571,10 +9592,10 @@
         <v>68</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>237</v>
+        <v>1966</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>1003</v>
+        <v>250</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -9582,10 +9603,10 @@
         <v>69</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>239</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -9593,10 +9614,10 @@
         <v>70</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>251</v>
+        <v>237</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -9604,10 +9625,10 @@
         <v>71</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>1713</v>
+        <v>238</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>1712</v>
+        <v>239</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -9615,10 +9636,10 @@
         <v>72</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>240</v>
+        <v>251</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -9626,10 +9647,10 @@
         <v>73</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>241</v>
+        <v>1713</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>1006</v>
+        <v>1712</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -9637,10 +9658,10 @@
         <v>74</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -9648,10 +9669,10 @@
         <v>75</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -9659,10 +9680,10 @@
         <v>76</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>1009</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -9670,10 +9691,10 @@
         <v>77</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>213</v>
+        <v>243</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>216</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -9681,10 +9702,10 @@
         <v>78</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>214</v>
+        <v>244</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>246</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -9692,10 +9713,10 @@
         <v>79</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -9703,10 +9724,10 @@
         <v>80</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>249</v>
+        <v>214</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -9714,10 +9735,10 @@
         <v>81</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>253</v>
+        <v>215</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -9725,10 +9746,10 @@
         <v>82</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>300</v>
+        <v>249</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>1010</v>
+        <v>248</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -9736,10 +9757,10 @@
         <v>83</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>301</v>
+        <v>253</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>1011</v>
+        <v>252</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -9747,10 +9768,10 @@
         <v>84</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -9758,10 +9779,10 @@
         <v>85</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>921</v>
+        <v>301</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>940</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -9769,10 +9790,10 @@
         <v>86</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>922</v>
+        <v>302</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>939</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -9780,10 +9801,10 @@
         <v>87</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>938</v>
+        <v>940</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -9791,10 +9812,10 @@
         <v>88</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>937</v>
+        <v>939</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -9802,10 +9823,10 @@
         <v>89</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>936</v>
+        <v>938</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -9813,10 +9834,10 @@
         <v>90</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>935</v>
+        <v>937</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -9824,10 +9845,10 @@
         <v>91</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>934</v>
+        <v>936</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -9835,10 +9856,10 @@
         <v>92</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>931</v>
+        <v>935</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -9846,10 +9867,10 @@
         <v>93</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>932</v>
+        <v>934</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -9857,10 +9878,10 @@
         <v>94</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -9868,10 +9889,10 @@
         <v>95</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>1997</v>
+        <v>929</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>1996</v>
+        <v>932</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -9879,10 +9900,10 @@
         <v>96</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>2000</v>
+        <v>930</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>1998</v>
+        <v>933</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -9890,21 +9911,33 @@
         <v>97</v>
       </c>
       <c r="B98" s="1" t="s">
+        <v>1997</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>1996</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="12">
+        <v>98</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>2000</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>1998</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="12">
+        <v>99</v>
+      </c>
+      <c r="B100" s="1" t="s">
         <v>2025</v>
       </c>
-      <c r="C98" s="1" t="s">
+      <c r="C100" s="1" t="s">
         <v>2024</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" s="1"/>
-      <c r="B99" s="1"/>
-      <c r="C99" s="1"/>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" s="1"/>
-      <c r="B100" s="1"/>
-      <c r="C100" s="1"/>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
@@ -9940,6 +9973,16 @@
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="1"/>
+      <c r="B108" s="1"/>
+      <c r="C108" s="1"/>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="1"/>
+      <c r="B109" s="1"/>
+      <c r="C109" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -10168,7 +10211,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>

</xml_diff>